<commit_message>
20191009 1815 SP recebe arquivo excel
</commit_message>
<xml_diff>
--- a/scripts/001 Procon Links DoNotCall.xlsx
+++ b/scripts/001 Procon Links DoNotCall.xlsx
@@ -62,9 +62,6 @@
     <t>SP</t>
   </si>
   <si>
-    <t>http://www.procon.sp.gov.br/BloqueioTelef/index.asp?modulo=fornecedor&amp;pagina=login</t>
-  </si>
-  <si>
     <t>http://www.bloqtel.ms.gov.br/fornecedorAcesso.aspx</t>
   </si>
   <si>
@@ -242,12 +239,6 @@
     <t>obs old</t>
   </si>
   <si>
-    <t>.xlsx</t>
-  </si>
-  <si>
-    <t>.xlsx // del linhas acima do cabeçalho // salvar</t>
-  </si>
-  <si>
     <t>.xlsx // del linhas acima do cabeçalho // retirar todas as mesclas // salvar</t>
   </si>
   <si>
@@ -260,13 +251,22 @@
     <t>.csv // apagar linhas acima do cabeçalho e rodape</t>
   </si>
   <si>
-    <t>zip //  .csv // apagar linhas acima do cabeçalho e rodape</t>
-  </si>
-  <si>
     <t>.csv</t>
   </si>
   <si>
     <t>.txt</t>
+  </si>
+  <si>
+    <t>https://bloqueio.procon.sp.gov.br/#/signIn/supplier</t>
+  </si>
+  <si>
+    <t>zip //  .xlsx // apagar linhas acima do cabeçalho e rodape</t>
+  </si>
+  <si>
+    <t>.xls --&gt; .xlsx // del linhas acima do cabeçalho</t>
+  </si>
+  <si>
+    <t>.xls --&gt; .xlsx // apagar linha em branco acima do cabeçalho</t>
   </si>
 </sst>
 </file>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,22 +735,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -761,33 +761,33 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="4">
         <v>915480</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
         <v>57</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -798,13 +798,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="4">
         <v>915480</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -812,16 +812,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>915480</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -846,36 +846,36 @@
         <v>8</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4">
         <v>915480</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="D8" s="4">
         <v>915480</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -886,34 +886,34 @@
         <v>9</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="4">
         <v>915480</v>
       </c>
       <c r="F9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4"/>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -924,13 +924,13 @@
         <v>11</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="4">
         <v>915480</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -938,16 +938,16 @@
         <v>13</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -955,42 +955,42 @@
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="4">
-        <v>915480</v>
+        <v>915481</v>
       </c>
       <c r="F13" t="s">
         <v>81</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1004,7 +1004,7 @@
     <hyperlink ref="C6" r:id="rId7"/>
     <hyperlink ref="B9" r:id="rId8"/>
     <hyperlink ref="B11" r:id="rId9"/>
-    <hyperlink ref="B13" r:id="rId10"/>
+    <hyperlink ref="B13" r:id="rId10" location="/signIn/supplier"/>
     <hyperlink ref="B17" r:id="rId11"/>
     <hyperlink ref="B10" r:id="rId12"/>
     <hyperlink ref="B3" r:id="rId13"/>
@@ -1036,12 +1036,12 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -1051,42 +1051,42 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1101,33 +1101,33 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>63</v>
-      </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
@@ -1142,30 +1142,30 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
         <v>51</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>52</v>
-      </c>
-      <c r="G17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -1175,34 +1175,34 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C22" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1212,12 +1212,12 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C24" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C25" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1232,21 +1232,21 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C29" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>